<commit_message>
export to scriptable object
</commit_message>
<xml_diff>
--- a/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Others.xlsx
+++ b/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Others.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="120" documentId="11_725AD12240320D347474AE0F146D62A3A4C91C0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DF7B807-E5D9-4F46-A16E-CB58B7286D53}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="11_725AD12240320D347474AE0F146D62A3A4C91C0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9529713B-6984-43F1-8962-9D343F1D2A20}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="5" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Id</t>
   </si>
@@ -267,12 +267,6 @@
   </si>
   <si>
     <t>Direct/Image01.png[Image01_3]</t>
-  </si>
-  <si>
-    <t>ASSET004</t>
-  </si>
-  <si>
-    <t>ASSET005</t>
   </si>
 </sst>
 </file>
@@ -389,7 +383,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -435,13 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1094,9 +1082,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1111,13 +1099,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="12" customFormat="1" ht="13.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -1134,13 +1122,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="14"/>
@@ -1153,16 +1141,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="6"/>
@@ -1174,13 +1162,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -1193,46 +1181,6 @@
         <v>12</v>
       </c>
       <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1343,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE73F2EC-2397-4281-93D2-074E147D83D4}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75"/>
@@ -1411,17 +1359,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5">
-      <c r="A5" s="11" t="s">
-        <v>77</v>
-      </c>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5">
-      <c r="A6" s="11" t="s">
-        <v>78</v>
-      </c>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
     </row>

</xml_diff>

<commit_message>
updating asset path spec
</commit_message>
<xml_diff>
--- a/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Others.xlsx
+++ b/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Others.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="121" documentId="11_725AD12240320D347474AE0F146D62A3A4C91C0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9529713B-6984-43F1-8962-9D343F1D2A20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{541376D7-CCB8-44AC-B962-DB68ABD09361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Direct/Image01.png[Image01_3]</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1295,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75"/>
@@ -1359,8 +1362,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11"/>
+    <row r="5" spans="1:4" ht="13.5">
+      <c r="A5" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>

</xml_diff>